<commit_message>
add easyrdf and phpexcel and test vocab exports
</commit_message>
<xml_diff>
--- a/storage/app/public/vocabs/analogue/1.3/analogue_1-3.xlsx
+++ b/storage/app/public/vocabs/analogue/1.3/analogue_1-3.xlsx
@@ -4068,15 +4068,19 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9949,7 +9953,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
@@ -9961,5 +9964,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>